<commit_message>
🗃️ (TST_Srinivasan_2021-11_QS): fix date
FIX #60
</commit_message>
<xml_diff>
--- a/Data/raw/TST_Srinivasan_2021-11_QS/TST_2021-11_QS_metadata.xlsx
+++ b/Data/raw/TST_Srinivasan_2021-11_QS/TST_2021-11_QS_metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment" sheetId="1" state="visible" r:id="rId2"/>
@@ -143,7 +143,7 @@
     <t xml:space="preserve">Dharun Vadugappatty Srinivasan</t>
   </si>
   <si>
-    <t xml:space="preserve">2020-11</t>
+    <t xml:space="preserve">2021-11</t>
   </si>
   <si>
     <t xml:space="preserve">QS</t>
@@ -307,7 +307,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -344,12 +344,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -415,7 +409,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -469,10 +463,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -499,8 +489,8 @@
   </sheetPr>
   <dimension ref="B1:AM1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="102" zoomScaleNormal="102" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="102" zoomScaleNormal="102" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -989,7 +979,7 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -1019,7 +1009,7 @@
       <c r="B1" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="1" t="s">
         <v>83</v>
       </c>
       <c r="D1" s="13" t="s">
@@ -1045,7 +1035,7 @@
       <c r="C2" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="15" t="n">
+      <c r="D2" s="14" t="n">
         <v>15</v>
       </c>
       <c r="E2" s="1"/>
@@ -1068,7 +1058,7 @@
       <c r="C3" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="15" t="n">
+      <c r="D3" s="14" t="n">
         <v>15</v>
       </c>
       <c r="E3" s="1"/>
@@ -1091,7 +1081,7 @@
       <c r="C4" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="15" t="n">
+      <c r="D4" s="14" t="n">
         <v>15</v>
       </c>
       <c r="E4" s="1"/>
@@ -1114,7 +1104,7 @@
       <c r="C5" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="15" t="n">
+      <c r="D5" s="14" t="n">
         <v>15</v>
       </c>
       <c r="E5" s="1"/>
@@ -1137,7 +1127,7 @@
       <c r="C6" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="15" t="n">
+      <c r="D6" s="14" t="n">
         <v>15</v>
       </c>
       <c r="E6" s="1"/>
@@ -1160,7 +1150,7 @@
       <c r="C7" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="15" t="n">
+      <c r="D7" s="14" t="n">
         <v>15</v>
       </c>
       <c r="E7" s="1"/>
@@ -1183,7 +1173,7 @@
       <c r="C8" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="15" t="n">
+      <c r="D8" s="14" t="n">
         <v>15</v>
       </c>
       <c r="E8" s="1"/>

</xml_diff>